<commit_message>
Create and set up the environment for the Paging test suites
</commit_message>
<xml_diff>
--- a/source/TestData/data.xlsx
+++ b/source/TestData/data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="paging" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>*** Test Cases ***</t>
   </si>
@@ -91,6 +92,51 @@
   </si>
   <si>
     <t>Right pass wrong user</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>${item}</t>
+  </si>
+  <si>
+    <t>Item on page 9</t>
+  </si>
+  <si>
+    <t>Item on page 18</t>
+  </si>
+  <si>
+    <t>Item on page 32</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Pagination: 18 items on a page</t>
+  </si>
+  <si>
+    <t>Pagination: 9 items on a page</t>
+  </si>
+  <si>
+    <t>Pagination: 32 items on a page</t>
+  </si>
+  <si>
+    <t>Pagination: All items on a page</t>
+  </si>
+  <si>
+    <t>Check there are 9 items on 1 page</t>
+  </si>
+  <si>
+    <t>Check there are 18 items on 1 page</t>
+  </si>
+  <si>
+    <t>Check there are 32 items on 1 page</t>
+  </si>
+  <si>
+    <t>Check there are all items on 1 page</t>
   </si>
 </sst>
 </file>
@@ -414,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,4 +600,110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="51.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Login test suite
</commit_message>
<xml_diff>
--- a/source/TestData/data.xlsx
+++ b/source/TestData/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>*** Test Cases ***</t>
   </si>
@@ -67,9 +67,6 @@
     <t>TC01</t>
   </si>
   <si>
-    <t>Please fill out this field.</t>
-  </si>
-  <si>
     <t>asd-1245</t>
   </si>
   <si>
@@ -137,6 +134,24 @@
   </si>
   <si>
     <t>Check there are all items on 1 page</t>
+  </si>
+  <si>
+    <t>//span[@id="Header_LoginViewHeader_LoginName1"]</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>//span[@id="PasswordRequired"]</t>
+  </si>
+  <si>
+    <t>//span[@id="UserNameRequired"]</t>
+  </si>
+  <si>
+    <t>${xpath}</t>
+  </si>
+  <si>
+    <t>//div[@class="text-danger"]</t>
   </si>
 </sst>
 </file>
@@ -172,11 +187,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,13 +490,14 @@
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="53.5546875" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,59 +508,68 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -546,17 +577,20 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -564,19 +598,22 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -586,13 +623,16 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -607,7 +647,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -637,70 +677,70 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>